<commit_message>
add doc about seleniumobj functions usage
</commit_message>
<xml_diff>
--- a/Selenium/Docs/SeleniumCommand.xlsx
+++ b/Selenium/Docs/SeleniumCommand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA79949-1A3D-43DD-80F0-3BE26CDFDB1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6988DB1D-2621-4AA7-858B-F2381770F450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="175">
   <si>
     <t>log_name</t>
   </si>
@@ -880,6 +880,227 @@
   </si>
   <si>
     <t>mathod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">id </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>send_keys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_attribute</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>xpath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xpaths</t>
+  </si>
+  <si>
+    <t>ids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>link_text</t>
+  </si>
+  <si>
+    <t>link_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>partial_link_text</t>
+  </si>
+  <si>
+    <t>partial_link_texts</t>
+  </si>
+  <si>
+    <t>partial_link_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>tag_name</t>
+  </si>
+  <si>
+    <t>tag_names</t>
+  </si>
+  <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>class_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class_names</t>
+  </si>
+  <si>
+    <t>css_selector</t>
+  </si>
+  <si>
+    <t>css_selector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>css_selectors</t>
+  </si>
+  <si>
+    <t>get_property</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击通过element元素定位到的元素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向通过element元素定位到的文本框输入字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回定位到的element元素的属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回定位到的element元素的类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空通过element元素定位到的文本框</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交表单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string/filepath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_by_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_by_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select_by_visible_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all_selected_options</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deselect_all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deselect_by_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deselect_by_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deselect_by_visible_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first_selected_option</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visible_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过索引选择定位到的下拉框内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过value选择定位到的下拉框内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过选项内容选择定位到的下拉框内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回所有被选择的下拉框选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空所有被选中的下拉框选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回第一个被选中的下拉框选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过visible_text取消选中的下拉框选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过value取消选中的下拉框选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过索引取消选中的下拉框选项</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1042,18 +1263,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1089,6 +1304,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1370,17 +1600,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132:E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.5546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="31.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="61.6640625" style="1" customWidth="1"/>
@@ -1393,13 +1623,13 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="9"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1408,46 +1638,46 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="6" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1464,7 +1694,7 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1481,15 +1711,13 @@
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F5" s="21"/>
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1504,15 +1732,13 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F6" s="21"/>
       <c r="H6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1524,15 +1750,13 @@
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F7" s="21"/>
       <c r="H7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1544,15 +1768,13 @@
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F8" s="21"/>
       <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1564,15 +1786,13 @@
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F9" s="21"/>
       <c r="H9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1584,15 +1804,13 @@
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F10" s="21"/>
       <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1604,15 +1822,13 @@
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F11" s="21"/>
       <c r="H11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1624,15 +1840,13 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F12" s="21"/>
       <c r="H12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1644,16 +1858,14 @@
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="12" t="s">
+      <c r="F13" s="21"/>
+      <c r="H13" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1664,15 +1876,13 @@
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F14" s="21"/>
       <c r="H14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1684,15 +1894,13 @@
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="21"/>
       <c r="H15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1704,15 +1912,13 @@
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F16" s="21"/>
       <c r="H16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1724,15 +1930,13 @@
       <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F17" s="21"/>
       <c r="H17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1744,15 +1948,13 @@
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F18" s="21"/>
       <c r="H18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1764,15 +1966,13 @@
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F19" s="21"/>
       <c r="G19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1787,15 +1987,13 @@
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F20" s="21"/>
       <c r="G20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1810,15 +2008,13 @@
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F21" s="21"/>
       <c r="H21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1830,15 +2026,13 @@
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F22" s="21"/>
       <c r="H22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1850,15 +2044,13 @@
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F23" s="21"/>
       <c r="H23" s="1" t="s">
         <v>63</v>
       </c>
@@ -1870,15 +2062,13 @@
       <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F24" s="21"/>
       <c r="G24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1893,15 +2083,13 @@
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F25" s="21"/>
       <c r="G25" s="1" t="s">
         <v>66</v>
       </c>
@@ -1916,15 +2104,13 @@
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F26" s="21"/>
       <c r="H26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1936,15 +2122,13 @@
       <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F27" s="21"/>
       <c r="G27" s="1" t="s">
         <v>74</v>
       </c>
@@ -1959,15 +2143,13 @@
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F28" s="21"/>
       <c r="G28" s="1" t="s">
         <v>80</v>
       </c>
@@ -1982,19 +2164,17 @@
       <c r="C29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F29" s="21"/>
       <c r="G29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="12" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2005,15 +2185,13 @@
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F30" s="21"/>
       <c r="G30" s="1" t="s">
         <v>80</v>
       </c>
@@ -2028,16 +2206,14 @@
       <c r="C31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="13" t="s">
+      <c r="F31" s="21"/>
+      <c r="G31" s="11" t="s">
         <v>85</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -2051,15 +2227,13 @@
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F32" s="21"/>
       <c r="H32" s="1" t="s">
         <v>89</v>
       </c>
@@ -2071,16 +2245,14 @@
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="13" t="s">
+      <c r="F33" s="21"/>
+      <c r="G33" s="11" t="s">
         <v>85</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -2094,15 +2266,13 @@
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="14" t="s">
         <v>92</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F34" s="21"/>
       <c r="H34" s="1" t="s">
         <v>86</v>
       </c>
@@ -2114,15 +2284,13 @@
       <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="H35" s="1" t="s">
         <v>94</v>
       </c>
@@ -2134,16 +2302,14 @@
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="9" t="s">
         <v>95</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="16" t="s">
+      <c r="F36" s="21"/>
+      <c r="G36" s="14" t="s">
         <v>97</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -2157,16 +2323,14 @@
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="13" t="s">
+      <c r="F37" s="21"/>
+      <c r="G37" s="11" t="s">
         <v>101</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -2180,19 +2344,17 @@
       <c r="C38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="9" t="s">
         <v>103</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="16" t="s">
+      <c r="F38" s="21"/>
+      <c r="G38" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="15" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2203,19 +2365,17 @@
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="13" t="s">
+      <c r="F39" s="21"/>
+      <c r="G39" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="16" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2226,16 +2386,14 @@
       <c r="C40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="9" t="s">
         <v>109</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="19" t="s">
+      <c r="F40" s="21"/>
+      <c r="H40" s="17" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2246,26 +2404,3103 @@
       <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="13" t="s">
+      <c r="F41" s="21"/>
+      <c r="G41" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="18" t="s">
         <v>112</v>
       </c>
     </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="20"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="20"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="20"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="20"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" s="20"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F72" s="21"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="20"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="20"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="B75" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D75" s="20"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D76" s="20"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="B77" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77" s="20"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="20"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" s="20"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+    </row>
+    <row r="80" spans="2:8">
+      <c r="B80" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" s="20"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+    </row>
+    <row r="81" spans="2:8">
+      <c r="B81" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D81" s="20"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+    </row>
+    <row r="82" spans="2:8">
+      <c r="B82" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D82" s="20"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+    </row>
+    <row r="83" spans="2:8">
+      <c r="B83" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="20"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+    </row>
+    <row r="84" spans="2:8">
+      <c r="B84" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D84" s="20"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="19"/>
+    </row>
+    <row r="85" spans="2:8">
+      <c r="B85" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+    </row>
+    <row r="86" spans="2:8">
+      <c r="B86" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="20"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+    </row>
+    <row r="87" spans="2:8">
+      <c r="B87" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F87" s="21"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8">
+      <c r="B88" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D88" s="20"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+    </row>
+    <row r="89" spans="2:8">
+      <c r="B89" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D89" s="20"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="20"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+    </row>
+    <row r="91" spans="2:8">
+      <c r="B91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+    </row>
+    <row r="92" spans="2:8">
+      <c r="B92" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="20"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+    </row>
+    <row r="93" spans="2:8">
+      <c r="B93" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D93" s="20"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="19"/>
+    </row>
+    <row r="94" spans="2:8">
+      <c r="B94" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D94" s="20"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="19"/>
+    </row>
+    <row r="95" spans="2:8">
+      <c r="B95" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D95" s="20"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
+    </row>
+    <row r="96" spans="2:8">
+      <c r="B96" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D96" s="20"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="19"/>
+    </row>
+    <row r="97" spans="2:8">
+      <c r="B97" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D97" s="20"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="19"/>
+    </row>
+    <row r="98" spans="2:8">
+      <c r="B98" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19"/>
+    </row>
+    <row r="99" spans="2:8">
+      <c r="B99" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D99" s="20"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19"/>
+    </row>
+    <row r="100" spans="2:8">
+      <c r="B100" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D100" s="20"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="19"/>
+    </row>
+    <row r="101" spans="2:8">
+      <c r="B101" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" s="20"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="19"/>
+    </row>
+    <row r="102" spans="2:8">
+      <c r="B102" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F102" s="21"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8">
+      <c r="B103" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" s="20"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+    </row>
+    <row r="104" spans="2:8">
+      <c r="B104" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D104" s="20"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+    </row>
+    <row r="105" spans="2:8">
+      <c r="B105" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D105" s="20"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="19"/>
+    </row>
+    <row r="106" spans="2:8">
+      <c r="B106" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D106" s="20"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="19"/>
+    </row>
+    <row r="107" spans="2:8">
+      <c r="B107" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D107" s="20"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+    </row>
+    <row r="108" spans="2:8">
+      <c r="B108" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D108" s="20"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+    </row>
+    <row r="109" spans="2:8">
+      <c r="B109" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+    </row>
+    <row r="110" spans="2:8">
+      <c r="B110" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D110" s="20"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+    </row>
+    <row r="111" spans="2:8">
+      <c r="B111" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D111" s="20"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="19"/>
+    </row>
+    <row r="112" spans="2:8">
+      <c r="B112" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D112" s="20"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+    </row>
+    <row r="113" spans="2:8">
+      <c r="B113" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D113" s="20"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
+    </row>
+    <row r="114" spans="2:8">
+      <c r="B114" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D114" s="20"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="21"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19"/>
+    </row>
+    <row r="115" spans="2:8">
+      <c r="B115" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D115" s="20"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="21"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="19"/>
+    </row>
+    <row r="116" spans="2:8">
+      <c r="B116" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D116" s="20"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="19"/>
+    </row>
+    <row r="117" spans="2:8">
+      <c r="B117" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E117" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F117" s="21"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="19"/>
+    </row>
+    <row r="118" spans="2:8">
+      <c r="B118" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D118" s="21"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="21"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8">
+      <c r="B119" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D119" s="21"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="19"/>
+    </row>
+    <row r="120" spans="2:8">
+      <c r="B120" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D120" s="21"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="19"/>
+    </row>
+    <row r="121" spans="2:8">
+      <c r="B121" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" s="21"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="21"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="19"/>
+    </row>
+    <row r="122" spans="2:8">
+      <c r="B122" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D122" s="21"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="19"/>
+      <c r="H122" s="19"/>
+    </row>
+    <row r="123" spans="2:8">
+      <c r="B123" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D123" s="21"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="21"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="19"/>
+    </row>
+    <row r="124" spans="2:8">
+      <c r="B124" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D124" s="21"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="19"/>
+    </row>
+    <row r="125" spans="2:8">
+      <c r="B125" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D125" s="21"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="19"/>
+      <c r="H125" s="19"/>
+    </row>
+    <row r="126" spans="2:8">
+      <c r="B126" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D126" s="21"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="19"/>
+      <c r="H126" s="19"/>
+    </row>
+    <row r="127" spans="2:8">
+      <c r="B127" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D127" s="21"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="19"/>
+      <c r="H127" s="19"/>
+    </row>
+    <row r="128" spans="2:8">
+      <c r="B128" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D128" s="21"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="21"/>
+      <c r="G128" s="19"/>
+      <c r="H128" s="19"/>
+    </row>
+    <row r="129" spans="2:8">
+      <c r="B129" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D129" s="21"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="21"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="19"/>
+    </row>
+    <row r="130" spans="2:8">
+      <c r="B130" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D130" s="21"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="21"/>
+      <c r="G130" s="19"/>
+      <c r="H130" s="19"/>
+    </row>
+    <row r="131" spans="2:8">
+      <c r="B131" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D131" s="21"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="21"/>
+      <c r="G131" s="19"/>
+      <c r="H131" s="19"/>
+    </row>
+    <row r="132" spans="2:8">
+      <c r="B132" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D132" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E132" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F132" s="21"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8">
+      <c r="B133" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D133" s="21"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="21"/>
+      <c r="G133" s="19"/>
+      <c r="H133" s="19"/>
+    </row>
+    <row r="134" spans="2:8">
+      <c r="B134" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C134" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D134" s="21"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="19"/>
+      <c r="H134" s="19"/>
+    </row>
+    <row r="135" spans="2:8">
+      <c r="B135" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C135" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D135" s="21"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="21"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="19"/>
+    </row>
+    <row r="136" spans="2:8">
+      <c r="B136" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D136" s="21"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="21"/>
+      <c r="G136" s="19"/>
+      <c r="H136" s="19"/>
+    </row>
+    <row r="137" spans="2:8">
+      <c r="B137" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D137" s="21"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="21"/>
+      <c r="G137" s="19"/>
+      <c r="H137" s="19"/>
+    </row>
+    <row r="138" spans="2:8">
+      <c r="B138" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D138" s="21"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="19"/>
+    </row>
+    <row r="139" spans="2:8">
+      <c r="B139" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D139" s="21"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="19"/>
+      <c r="H139" s="19"/>
+    </row>
+    <row r="140" spans="2:8">
+      <c r="B140" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D140" s="21"/>
+      <c r="E140" s="19"/>
+      <c r="F140" s="21"/>
+      <c r="G140" s="19"/>
+      <c r="H140" s="19"/>
+    </row>
+    <row r="141" spans="2:8">
+      <c r="B141" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D141" s="21"/>
+      <c r="E141" s="19"/>
+      <c r="F141" s="21"/>
+      <c r="G141" s="19"/>
+      <c r="H141" s="19"/>
+    </row>
+    <row r="142" spans="2:8">
+      <c r="B142" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D142" s="21"/>
+      <c r="E142" s="19"/>
+      <c r="F142" s="21"/>
+      <c r="G142" s="19"/>
+      <c r="H142" s="19"/>
+    </row>
+    <row r="143" spans="2:8">
+      <c r="B143" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D143" s="21"/>
+      <c r="E143" s="19"/>
+      <c r="F143" s="21"/>
+      <c r="G143" s="19"/>
+      <c r="H143" s="19"/>
+    </row>
+    <row r="144" spans="2:8">
+      <c r="B144" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D144" s="21"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="19"/>
+      <c r="H144" s="19"/>
+    </row>
+    <row r="145" spans="2:8">
+      <c r="B145" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D145" s="21"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="21"/>
+      <c r="G145" s="19"/>
+      <c r="H145" s="19"/>
+    </row>
+    <row r="146" spans="2:8">
+      <c r="B146" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D146" s="21"/>
+      <c r="E146" s="19"/>
+      <c r="F146" s="21"/>
+      <c r="G146" s="19"/>
+      <c r="H146" s="19"/>
+    </row>
+    <row r="147" spans="2:8">
+      <c r="B147" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D147" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E147" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F147" s="21"/>
+      <c r="G147" s="19"/>
+      <c r="H147" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8">
+      <c r="B148" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D148" s="21"/>
+      <c r="E148" s="19"/>
+      <c r="F148" s="21"/>
+      <c r="G148" s="19"/>
+      <c r="H148" s="19"/>
+    </row>
+    <row r="149" spans="2:8">
+      <c r="B149" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D149" s="21"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="19"/>
+      <c r="H149" s="19"/>
+    </row>
+    <row r="150" spans="2:8">
+      <c r="B150" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D150" s="21"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="21"/>
+      <c r="G150" s="19"/>
+      <c r="H150" s="19"/>
+    </row>
+    <row r="151" spans="2:8">
+      <c r="B151" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D151" s="21"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="19"/>
+      <c r="H151" s="19"/>
+    </row>
+    <row r="152" spans="2:8">
+      <c r="B152" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D152" s="21"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="21"/>
+      <c r="G152" s="19"/>
+      <c r="H152" s="19"/>
+    </row>
+    <row r="153" spans="2:8">
+      <c r="B153" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D153" s="21"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="19"/>
+      <c r="H153" s="19"/>
+    </row>
+    <row r="154" spans="2:8">
+      <c r="B154" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D154" s="21"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="19"/>
+      <c r="H154" s="19"/>
+    </row>
+    <row r="155" spans="2:8">
+      <c r="B155" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D155" s="21"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="21"/>
+      <c r="G155" s="19"/>
+      <c r="H155" s="19"/>
+    </row>
+    <row r="156" spans="2:8">
+      <c r="B156" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D156" s="21"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="21"/>
+      <c r="G156" s="19"/>
+      <c r="H156" s="19"/>
+    </row>
+    <row r="157" spans="2:8">
+      <c r="B157" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D157" s="21"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="21"/>
+      <c r="G157" s="19"/>
+      <c r="H157" s="19"/>
+    </row>
+    <row r="158" spans="2:8">
+      <c r="B158" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D158" s="21"/>
+      <c r="E158" s="19"/>
+      <c r="F158" s="21"/>
+      <c r="G158" s="19"/>
+      <c r="H158" s="19"/>
+    </row>
+    <row r="159" spans="2:8">
+      <c r="B159" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D159" s="21"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="19"/>
+      <c r="H159" s="19"/>
+    </row>
+    <row r="160" spans="2:8">
+      <c r="B160" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D160" s="21"/>
+      <c r="E160" s="19"/>
+      <c r="F160" s="21"/>
+      <c r="G160" s="19"/>
+      <c r="H160" s="19"/>
+    </row>
+    <row r="161" spans="2:8">
+      <c r="B161" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D161" s="21"/>
+      <c r="E161" s="19"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="19"/>
+      <c r="H161" s="19"/>
+    </row>
+    <row r="162" spans="2:8">
+      <c r="B162" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D162" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E162" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F162" s="21"/>
+      <c r="G162" s="19"/>
+      <c r="H162" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8">
+      <c r="B163" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D163" s="21"/>
+      <c r="E163" s="19"/>
+      <c r="F163" s="21"/>
+      <c r="G163" s="19"/>
+      <c r="H163" s="19"/>
+    </row>
+    <row r="164" spans="2:8">
+      <c r="B164" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D164" s="21"/>
+      <c r="E164" s="19"/>
+      <c r="F164" s="21"/>
+      <c r="G164" s="19"/>
+      <c r="H164" s="19"/>
+    </row>
+    <row r="165" spans="2:8">
+      <c r="B165" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D165" s="21"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="21"/>
+      <c r="G165" s="19"/>
+      <c r="H165" s="19"/>
+    </row>
+    <row r="166" spans="2:8">
+      <c r="B166" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D166" s="21"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="21"/>
+      <c r="G166" s="19"/>
+      <c r="H166" s="19"/>
+    </row>
+    <row r="167" spans="2:8">
+      <c r="B167" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D167" s="21"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="21"/>
+      <c r="G167" s="19"/>
+      <c r="H167" s="19"/>
+    </row>
+    <row r="168" spans="2:8">
+      <c r="B168" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D168" s="21"/>
+      <c r="E168" s="19"/>
+      <c r="F168" s="21"/>
+      <c r="G168" s="19"/>
+      <c r="H168" s="19"/>
+    </row>
+    <row r="169" spans="2:8">
+      <c r="B169" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D169" s="21"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="21"/>
+      <c r="G169" s="19"/>
+      <c r="H169" s="19"/>
+    </row>
+    <row r="170" spans="2:8">
+      <c r="B170" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D170" s="21"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="21"/>
+      <c r="G170" s="19"/>
+      <c r="H170" s="19"/>
+    </row>
+    <row r="171" spans="2:8">
+      <c r="B171" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D171" s="21"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="21"/>
+      <c r="G171" s="19"/>
+      <c r="H171" s="19"/>
+    </row>
+    <row r="172" spans="2:8">
+      <c r="B172" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C172" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D172" s="21"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="21"/>
+      <c r="G172" s="19"/>
+      <c r="H172" s="19"/>
+    </row>
+    <row r="173" spans="2:8">
+      <c r="B173" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D173" s="21"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="21"/>
+      <c r="G173" s="19"/>
+      <c r="H173" s="19"/>
+    </row>
+    <row r="174" spans="2:8">
+      <c r="B174" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D174" s="21"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="21"/>
+      <c r="G174" s="19"/>
+      <c r="H174" s="19"/>
+    </row>
+    <row r="175" spans="2:8">
+      <c r="B175" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D175" s="21"/>
+      <c r="E175" s="19"/>
+      <c r="F175" s="21"/>
+      <c r="G175" s="19"/>
+      <c r="H175" s="19"/>
+    </row>
+    <row r="176" spans="2:8">
+      <c r="B176" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D176" s="21"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="21"/>
+      <c r="G176" s="19"/>
+      <c r="H176" s="19"/>
+    </row>
+    <row r="177" spans="2:8">
+      <c r="B177" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D177" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E177" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F177" s="21"/>
+      <c r="G177" s="19"/>
+      <c r="H177" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8">
+      <c r="B178" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D178" s="21"/>
+      <c r="E178" s="19"/>
+      <c r="F178" s="21"/>
+      <c r="G178" s="19"/>
+      <c r="H178" s="19"/>
+    </row>
+    <row r="179" spans="2:8">
+      <c r="B179" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D179" s="21"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="21"/>
+      <c r="G179" s="19"/>
+      <c r="H179" s="19"/>
+    </row>
+    <row r="180" spans="2:8">
+      <c r="B180" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D180" s="21"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="21"/>
+      <c r="G180" s="19"/>
+      <c r="H180" s="19"/>
+    </row>
+    <row r="181" spans="2:8">
+      <c r="B181" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C181" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D181" s="21"/>
+      <c r="E181" s="19"/>
+      <c r="F181" s="21"/>
+      <c r="G181" s="19"/>
+      <c r="H181" s="19"/>
+    </row>
+    <row r="182" spans="2:8">
+      <c r="B182" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D182" s="21"/>
+      <c r="E182" s="19"/>
+      <c r="F182" s="21"/>
+      <c r="G182" s="19"/>
+      <c r="H182" s="19"/>
+    </row>
+    <row r="183" spans="2:8">
+      <c r="B183" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D183" s="21"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="21"/>
+      <c r="G183" s="19"/>
+      <c r="H183" s="19"/>
+    </row>
+    <row r="184" spans="2:8">
+      <c r="B184" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D184" s="21"/>
+      <c r="E184" s="19"/>
+      <c r="F184" s="21"/>
+      <c r="G184" s="19"/>
+      <c r="H184" s="19"/>
+    </row>
+    <row r="185" spans="2:8">
+      <c r="B185" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D185" s="21"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="21"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="19"/>
+    </row>
+    <row r="186" spans="2:8">
+      <c r="B186" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D186" s="21"/>
+      <c r="E186" s="19"/>
+      <c r="F186" s="21"/>
+      <c r="G186" s="19"/>
+      <c r="H186" s="19"/>
+    </row>
+    <row r="187" spans="2:8">
+      <c r="B187" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D187" s="21"/>
+      <c r="E187" s="19"/>
+      <c r="F187" s="21"/>
+      <c r="G187" s="19"/>
+      <c r="H187" s="19"/>
+    </row>
+    <row r="188" spans="2:8">
+      <c r="B188" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D188" s="21"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="21"/>
+      <c r="G188" s="19"/>
+      <c r="H188" s="19"/>
+    </row>
+    <row r="189" spans="2:8">
+      <c r="B189" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D189" s="21"/>
+      <c r="E189" s="19"/>
+      <c r="F189" s="21"/>
+      <c r="G189" s="19"/>
+      <c r="H189" s="19"/>
+    </row>
+    <row r="190" spans="2:8">
+      <c r="B190" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D190" s="21"/>
+      <c r="E190" s="19"/>
+      <c r="F190" s="21"/>
+      <c r="G190" s="19"/>
+      <c r="H190" s="19"/>
+    </row>
+    <row r="191" spans="2:8">
+      <c r="B191" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D191" s="21"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="21"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="19"/>
+    </row>
+    <row r="192" spans="2:8">
+      <c r="B192" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D192" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E192" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F192" s="21"/>
+      <c r="G192" s="19"/>
+      <c r="H192" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="193" spans="2:8">
+      <c r="B193" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D193" s="21"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="21"/>
+      <c r="G193" s="19"/>
+      <c r="H193" s="19"/>
+    </row>
+    <row r="194" spans="2:8">
+      <c r="B194" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D194" s="21"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="21"/>
+      <c r="G194" s="19"/>
+      <c r="H194" s="19"/>
+    </row>
+    <row r="195" spans="2:8">
+      <c r="B195" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D195" s="21"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="21"/>
+      <c r="G195" s="19"/>
+      <c r="H195" s="19"/>
+    </row>
+    <row r="196" spans="2:8">
+      <c r="B196" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C196" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D196" s="21"/>
+      <c r="E196" s="19"/>
+      <c r="F196" s="21"/>
+      <c r="G196" s="19"/>
+      <c r="H196" s="19"/>
+    </row>
+    <row r="197" spans="2:8">
+      <c r="B197" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D197" s="21"/>
+      <c r="E197" s="19"/>
+      <c r="F197" s="21"/>
+      <c r="G197" s="19"/>
+      <c r="H197" s="19"/>
+    </row>
+    <row r="198" spans="2:8">
+      <c r="B198" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D198" s="21"/>
+      <c r="E198" s="19"/>
+      <c r="F198" s="21"/>
+      <c r="G198" s="19"/>
+      <c r="H198" s="19"/>
+    </row>
+    <row r="199" spans="2:8">
+      <c r="B199" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C199" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D199" s="21"/>
+      <c r="E199" s="19"/>
+      <c r="F199" s="21"/>
+      <c r="G199" s="19"/>
+      <c r="H199" s="19"/>
+    </row>
+    <row r="200" spans="2:8">
+      <c r="B200" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D200" s="21"/>
+      <c r="E200" s="19"/>
+      <c r="F200" s="21"/>
+      <c r="G200" s="19"/>
+      <c r="H200" s="19"/>
+    </row>
+    <row r="201" spans="2:8">
+      <c r="B201" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D201" s="21"/>
+      <c r="E201" s="19"/>
+      <c r="F201" s="21"/>
+      <c r="G201" s="19"/>
+      <c r="H201" s="19"/>
+    </row>
+    <row r="202" spans="2:8">
+      <c r="B202" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C202" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D202" s="21"/>
+      <c r="E202" s="19"/>
+      <c r="F202" s="21"/>
+      <c r="G202" s="19"/>
+      <c r="H202" s="19"/>
+    </row>
+    <row r="203" spans="2:8">
+      <c r="B203" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C203" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D203" s="21"/>
+      <c r="E203" s="19"/>
+      <c r="F203" s="21"/>
+      <c r="G203" s="19"/>
+      <c r="H203" s="19"/>
+    </row>
+    <row r="204" spans="2:8">
+      <c r="B204" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C204" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D204" s="21"/>
+      <c r="E204" s="19"/>
+      <c r="F204" s="21"/>
+      <c r="G204" s="19"/>
+      <c r="H204" s="19"/>
+    </row>
+    <row r="205" spans="2:8">
+      <c r="B205" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D205" s="21"/>
+      <c r="E205" s="19"/>
+      <c r="F205" s="21"/>
+      <c r="G205" s="19"/>
+      <c r="H205" s="19"/>
+    </row>
+    <row r="206" spans="2:8">
+      <c r="B206" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C206" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D206" s="21"/>
+      <c r="E206" s="19"/>
+      <c r="F206" s="21"/>
+      <c r="G206" s="19"/>
+      <c r="H206" s="19"/>
+    </row>
+    <row r="207" spans="2:8">
+      <c r="B207" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D207" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E207" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F207" s="21"/>
+      <c r="G207" s="19"/>
+      <c r="H207" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="208" spans="2:8">
+      <c r="B208" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D208" s="21"/>
+      <c r="E208" s="19"/>
+      <c r="F208" s="21"/>
+      <c r="G208" s="19"/>
+      <c r="H208" s="19"/>
+    </row>
+    <row r="209" spans="2:8">
+      <c r="B209" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C209" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D209" s="21"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="21"/>
+      <c r="G209" s="19"/>
+      <c r="H209" s="19"/>
+    </row>
+    <row r="210" spans="2:8">
+      <c r="B210" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D210" s="21"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="21"/>
+      <c r="G210" s="19"/>
+      <c r="H210" s="19"/>
+    </row>
+    <row r="211" spans="2:8">
+      <c r="B211" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C211" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D211" s="21"/>
+      <c r="E211" s="19"/>
+      <c r="F211" s="21"/>
+      <c r="G211" s="19"/>
+      <c r="H211" s="19"/>
+    </row>
+    <row r="212" spans="2:8">
+      <c r="B212" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C212" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D212" s="21"/>
+      <c r="E212" s="19"/>
+      <c r="F212" s="21"/>
+      <c r="G212" s="19"/>
+      <c r="H212" s="19"/>
+    </row>
+    <row r="213" spans="2:8">
+      <c r="B213" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D213" s="21"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="21"/>
+      <c r="G213" s="19"/>
+      <c r="H213" s="19"/>
+    </row>
+    <row r="214" spans="2:8">
+      <c r="B214" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C214" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D214" s="21"/>
+      <c r="E214" s="19"/>
+      <c r="F214" s="21"/>
+      <c r="G214" s="19"/>
+      <c r="H214" s="19"/>
+    </row>
+    <row r="215" spans="2:8">
+      <c r="B215" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C215" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D215" s="21"/>
+      <c r="E215" s="19"/>
+      <c r="F215" s="21"/>
+      <c r="G215" s="19"/>
+      <c r="H215" s="19"/>
+    </row>
+    <row r="216" spans="2:8">
+      <c r="B216" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C216" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D216" s="21"/>
+      <c r="E216" s="19"/>
+      <c r="F216" s="21"/>
+      <c r="G216" s="19"/>
+      <c r="H216" s="19"/>
+    </row>
+    <row r="217" spans="2:8">
+      <c r="B217" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D217" s="21"/>
+      <c r="E217" s="19"/>
+      <c r="F217" s="21"/>
+      <c r="G217" s="19"/>
+      <c r="H217" s="19"/>
+    </row>
+    <row r="218" spans="2:8">
+      <c r="B218" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D218" s="21"/>
+      <c r="E218" s="19"/>
+      <c r="F218" s="21"/>
+      <c r="G218" s="19"/>
+      <c r="H218" s="19"/>
+    </row>
+    <row r="219" spans="2:8">
+      <c r="B219" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C219" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D219" s="21"/>
+      <c r="E219" s="19"/>
+      <c r="F219" s="21"/>
+      <c r="G219" s="19"/>
+      <c r="H219" s="19"/>
+    </row>
+    <row r="220" spans="2:8">
+      <c r="B220" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C220" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D220" s="21"/>
+      <c r="E220" s="19"/>
+      <c r="F220" s="21"/>
+      <c r="G220" s="19"/>
+      <c r="H220" s="19"/>
+    </row>
+    <row r="221" spans="2:8">
+      <c r="B221" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C221" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D221" s="21"/>
+      <c r="E221" s="19"/>
+      <c r="F221" s="21"/>
+      <c r="G221" s="19"/>
+      <c r="H221" s="19"/>
+    </row>
+    <row r="222" spans="2:8">
+      <c r="B222" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D222" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E222" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F222" s="21"/>
+      <c r="G222" s="19"/>
+      <c r="H222" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="223" spans="2:8">
+      <c r="B223" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D223" s="21"/>
+      <c r="E223" s="19"/>
+      <c r="F223" s="21"/>
+      <c r="G223" s="19"/>
+      <c r="H223" s="19"/>
+    </row>
+    <row r="224" spans="2:8">
+      <c r="B224" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C224" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D224" s="21"/>
+      <c r="E224" s="19"/>
+      <c r="F224" s="21"/>
+      <c r="G224" s="19"/>
+      <c r="H224" s="19"/>
+    </row>
+    <row r="225" spans="2:8">
+      <c r="B225" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C225" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D225" s="21"/>
+      <c r="E225" s="19"/>
+      <c r="F225" s="21"/>
+      <c r="G225" s="19"/>
+      <c r="H225" s="19"/>
+    </row>
+    <row r="226" spans="2:8">
+      <c r="B226" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D226" s="21"/>
+      <c r="E226" s="19"/>
+      <c r="F226" s="21"/>
+      <c r="G226" s="19"/>
+      <c r="H226" s="19"/>
+    </row>
+    <row r="227" spans="2:8">
+      <c r="B227" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C227" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D227" s="21"/>
+      <c r="E227" s="19"/>
+      <c r="F227" s="21"/>
+      <c r="G227" s="19"/>
+      <c r="H227" s="19"/>
+    </row>
+    <row r="228" spans="2:8">
+      <c r="B228" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D228" s="21"/>
+      <c r="E228" s="19"/>
+      <c r="F228" s="21"/>
+      <c r="G228" s="19"/>
+      <c r="H228" s="19"/>
+    </row>
+    <row r="229" spans="2:8">
+      <c r="B229" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C229" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D229" s="21"/>
+      <c r="E229" s="19"/>
+      <c r="F229" s="21"/>
+      <c r="G229" s="19"/>
+      <c r="H229" s="19"/>
+    </row>
+    <row r="230" spans="2:8">
+      <c r="B230" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C230" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D230" s="21"/>
+      <c r="E230" s="19"/>
+      <c r="F230" s="21"/>
+      <c r="G230" s="19"/>
+      <c r="H230" s="19"/>
+    </row>
+    <row r="231" spans="2:8">
+      <c r="B231" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D231" s="21"/>
+      <c r="E231" s="19"/>
+      <c r="F231" s="21"/>
+      <c r="G231" s="19"/>
+      <c r="H231" s="19"/>
+    </row>
+    <row r="232" spans="2:8">
+      <c r="B232" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C232" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D232" s="21"/>
+      <c r="E232" s="19"/>
+      <c r="F232" s="21"/>
+      <c r="G232" s="19"/>
+      <c r="H232" s="19"/>
+    </row>
+    <row r="233" spans="2:8">
+      <c r="B233" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C233" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D233" s="21"/>
+      <c r="E233" s="19"/>
+      <c r="F233" s="21"/>
+      <c r="G233" s="19"/>
+      <c r="H233" s="19"/>
+    </row>
+    <row r="234" spans="2:8">
+      <c r="B234" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D234" s="21"/>
+      <c r="E234" s="19"/>
+      <c r="F234" s="21"/>
+      <c r="G234" s="19"/>
+      <c r="H234" s="19"/>
+    </row>
+    <row r="235" spans="2:8">
+      <c r="B235" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D235" s="21"/>
+      <c r="E235" s="19"/>
+      <c r="F235" s="21"/>
+      <c r="G235" s="19"/>
+      <c r="H235" s="19"/>
+    </row>
+    <row r="236" spans="2:8">
+      <c r="B236" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C236" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D236" s="21"/>
+      <c r="E236" s="19"/>
+      <c r="F236" s="21"/>
+      <c r="G236" s="19"/>
+      <c r="H236" s="19"/>
+    </row>
+    <row r="237" spans="2:8">
+      <c r="B237" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D237" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E237" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F237" s="21"/>
+      <c r="G237" s="19"/>
+      <c r="H237" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="238" spans="2:8">
+      <c r="B238" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D238" s="21"/>
+      <c r="E238" s="19"/>
+      <c r="F238" s="21"/>
+      <c r="G238" s="19"/>
+      <c r="H238" s="19"/>
+    </row>
+    <row r="239" spans="2:8">
+      <c r="B239" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C239" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D239" s="21"/>
+      <c r="E239" s="19"/>
+      <c r="F239" s="21"/>
+      <c r="G239" s="19"/>
+      <c r="H239" s="19"/>
+    </row>
+    <row r="240" spans="2:8">
+      <c r="B240" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C240" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D240" s="21"/>
+      <c r="E240" s="19"/>
+      <c r="F240" s="21"/>
+      <c r="G240" s="19"/>
+      <c r="H240" s="19"/>
+    </row>
+    <row r="241" spans="2:8">
+      <c r="B241" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D241" s="21"/>
+      <c r="E241" s="19"/>
+      <c r="F241" s="21"/>
+      <c r="G241" s="19"/>
+      <c r="H241" s="19"/>
+    </row>
+    <row r="242" spans="2:8">
+      <c r="B242" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C242" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D242" s="21"/>
+      <c r="E242" s="19"/>
+      <c r="F242" s="21"/>
+      <c r="G242" s="19"/>
+      <c r="H242" s="19"/>
+    </row>
+    <row r="243" spans="2:8">
+      <c r="B243" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C243" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D243" s="21"/>
+      <c r="E243" s="19"/>
+      <c r="F243" s="21"/>
+      <c r="G243" s="19"/>
+      <c r="H243" s="19"/>
+    </row>
+    <row r="244" spans="2:8">
+      <c r="B244" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C244" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D244" s="21"/>
+      <c r="E244" s="19"/>
+      <c r="F244" s="21"/>
+      <c r="G244" s="19"/>
+      <c r="H244" s="19"/>
+    </row>
+    <row r="245" spans="2:8">
+      <c r="B245" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D245" s="21"/>
+      <c r="E245" s="19"/>
+      <c r="F245" s="21"/>
+      <c r="G245" s="19"/>
+      <c r="H245" s="19"/>
+    </row>
+    <row r="246" spans="2:8">
+      <c r="B246" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D246" s="21"/>
+      <c r="E246" s="19"/>
+      <c r="F246" s="21"/>
+      <c r="G246" s="19"/>
+      <c r="H246" s="19"/>
+    </row>
+    <row r="247" spans="2:8">
+      <c r="B247" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D247" s="21"/>
+      <c r="E247" s="19"/>
+      <c r="F247" s="21"/>
+      <c r="G247" s="19"/>
+      <c r="H247" s="19"/>
+    </row>
+    <row r="248" spans="2:8">
+      <c r="B248" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D248" s="21"/>
+      <c r="E248" s="19"/>
+      <c r="F248" s="21"/>
+      <c r="G248" s="19"/>
+      <c r="H248" s="19"/>
+    </row>
+    <row r="249" spans="2:8">
+      <c r="B249" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C249" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D249" s="21"/>
+      <c r="E249" s="19"/>
+      <c r="F249" s="21"/>
+      <c r="G249" s="19"/>
+      <c r="H249" s="19"/>
+    </row>
+    <row r="250" spans="2:8">
+      <c r="B250" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C250" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D250" s="21"/>
+      <c r="E250" s="19"/>
+      <c r="F250" s="21"/>
+      <c r="G250" s="19"/>
+      <c r="H250" s="19"/>
+    </row>
+    <row r="251" spans="2:8">
+      <c r="B251" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C251" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D251" s="21"/>
+      <c r="E251" s="19"/>
+      <c r="F251" s="21"/>
+      <c r="G251" s="19"/>
+      <c r="H251" s="19"/>
+    </row>
+    <row r="252" spans="2:8">
+      <c r="B252" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D252" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E252" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F252" s="21"/>
+      <c r="G252" s="19"/>
+      <c r="H252" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="253" spans="2:8">
+      <c r="B253" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D253" s="21"/>
+      <c r="E253" s="19"/>
+      <c r="F253" s="21"/>
+      <c r="G253" s="19"/>
+      <c r="H253" s="19"/>
+    </row>
+    <row r="254" spans="2:8">
+      <c r="B254" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C254" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D254" s="21"/>
+      <c r="E254" s="19"/>
+      <c r="F254" s="21"/>
+      <c r="G254" s="19"/>
+      <c r="H254" s="19"/>
+    </row>
+    <row r="255" spans="2:8">
+      <c r="B255" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C255" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D255" s="21"/>
+      <c r="E255" s="19"/>
+      <c r="F255" s="21"/>
+      <c r="G255" s="19"/>
+      <c r="H255" s="19"/>
+    </row>
+    <row r="256" spans="2:8">
+      <c r="B256" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C256" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D256" s="21"/>
+      <c r="E256" s="19"/>
+      <c r="F256" s="21"/>
+      <c r="G256" s="19"/>
+      <c r="H256" s="19"/>
+    </row>
+    <row r="257" spans="2:8">
+      <c r="B257" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C257" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D257" s="21"/>
+      <c r="E257" s="19"/>
+      <c r="F257" s="21"/>
+      <c r="G257" s="19"/>
+      <c r="H257" s="19"/>
+    </row>
+    <row r="258" spans="2:8">
+      <c r="B258" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C258" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D258" s="21"/>
+      <c r="E258" s="19"/>
+      <c r="F258" s="21"/>
+      <c r="G258" s="19"/>
+      <c r="H258" s="19"/>
+    </row>
+    <row r="259" spans="2:8">
+      <c r="B259" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C259" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D259" s="21"/>
+      <c r="E259" s="19"/>
+      <c r="F259" s="21"/>
+      <c r="G259" s="19"/>
+      <c r="H259" s="19"/>
+    </row>
+    <row r="260" spans="2:8">
+      <c r="B260" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C260" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D260" s="21"/>
+      <c r="E260" s="19"/>
+      <c r="F260" s="21"/>
+      <c r="G260" s="19"/>
+      <c r="H260" s="19"/>
+    </row>
+    <row r="261" spans="2:8">
+      <c r="B261" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C261" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D261" s="21"/>
+      <c r="E261" s="19"/>
+      <c r="F261" s="21"/>
+      <c r="G261" s="19"/>
+      <c r="H261" s="19"/>
+    </row>
+    <row r="262" spans="2:8">
+      <c r="B262" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C262" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D262" s="21"/>
+      <c r="E262" s="19"/>
+      <c r="F262" s="21"/>
+      <c r="G262" s="19"/>
+      <c r="H262" s="19"/>
+    </row>
+    <row r="263" spans="2:8">
+      <c r="B263" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C263" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D263" s="21"/>
+      <c r="E263" s="19"/>
+      <c r="F263" s="21"/>
+      <c r="G263" s="19"/>
+      <c r="H263" s="19"/>
+    </row>
+    <row r="264" spans="2:8">
+      <c r="B264" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C264" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D264" s="21"/>
+      <c r="E264" s="19"/>
+      <c r="F264" s="21"/>
+      <c r="G264" s="19"/>
+      <c r="H264" s="19"/>
+    </row>
+    <row r="265" spans="2:8">
+      <c r="B265" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C265" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D265" s="21"/>
+      <c r="E265" s="19"/>
+      <c r="F265" s="21"/>
+      <c r="G265" s="19"/>
+      <c r="H265" s="19"/>
+    </row>
+    <row r="266" spans="2:8">
+      <c r="B266" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C266" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D266" s="21"/>
+      <c r="E266" s="19"/>
+      <c r="F266" s="21"/>
+      <c r="G266" s="19"/>
+      <c r="H266" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="64">
+    <mergeCell ref="H237:H251"/>
+    <mergeCell ref="H252:H266"/>
+    <mergeCell ref="G252:G266"/>
+    <mergeCell ref="G237:G251"/>
+    <mergeCell ref="G222:G236"/>
+    <mergeCell ref="G132:G146"/>
+    <mergeCell ref="H132:H146"/>
+    <mergeCell ref="H147:H161"/>
+    <mergeCell ref="H162:H176"/>
+    <mergeCell ref="G162:G176"/>
+    <mergeCell ref="G147:G161"/>
+    <mergeCell ref="H177:H191"/>
+    <mergeCell ref="H192:H206"/>
+    <mergeCell ref="H207:H221"/>
+    <mergeCell ref="G207:G221"/>
+    <mergeCell ref="G192:G206"/>
+    <mergeCell ref="G177:G191"/>
+    <mergeCell ref="D252:D266"/>
+    <mergeCell ref="E252:E266"/>
+    <mergeCell ref="F42:F266"/>
+    <mergeCell ref="D222:D236"/>
+    <mergeCell ref="E222:E236"/>
+    <mergeCell ref="D237:D251"/>
+    <mergeCell ref="E237:E251"/>
+    <mergeCell ref="H222:H236"/>
+    <mergeCell ref="D192:D206"/>
+    <mergeCell ref="E192:E206"/>
+    <mergeCell ref="D207:D221"/>
+    <mergeCell ref="E207:E221"/>
+    <mergeCell ref="D162:D176"/>
+    <mergeCell ref="E162:E176"/>
+    <mergeCell ref="D177:D191"/>
+    <mergeCell ref="E177:E191"/>
+    <mergeCell ref="D132:D146"/>
+    <mergeCell ref="E132:E146"/>
+    <mergeCell ref="D147:D161"/>
+    <mergeCell ref="E147:E161"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D42:D56"/>
+    <mergeCell ref="D57:D71"/>
+    <mergeCell ref="D72:D86"/>
+    <mergeCell ref="D87:D101"/>
+    <mergeCell ref="D102:D116"/>
+    <mergeCell ref="D117:D131"/>
+    <mergeCell ref="F4:F41"/>
+    <mergeCell ref="E42:E56"/>
+    <mergeCell ref="E57:E71"/>
+    <mergeCell ref="E72:E86"/>
+    <mergeCell ref="E87:E101"/>
+    <mergeCell ref="E102:E116"/>
+    <mergeCell ref="E117:E131"/>
+    <mergeCell ref="G42:G56"/>
+    <mergeCell ref="H42:H56"/>
+    <mergeCell ref="G57:G71"/>
+    <mergeCell ref="H57:H71"/>
+    <mergeCell ref="G72:G86"/>
+    <mergeCell ref="H72:H86"/>
+    <mergeCell ref="G118:G131"/>
+    <mergeCell ref="H118:H131"/>
+    <mergeCell ref="G87:G101"/>
+    <mergeCell ref="H87:H101"/>
+    <mergeCell ref="H102:H117"/>
+    <mergeCell ref="G102:G117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>